<commit_message>
Regroupement Année et Trimestre en colonne Période
</commit_message>
<xml_diff>
--- a/docs/referentiel_sources_chomage.xlsx
+++ b/docs/referentiel_sources_chomage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julie\Desktop\01. Fil Rouge\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E34F021-1BEB-49D9-84FF-6FD089E68D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01EBC026-4FED-40A5-9FB8-E3553E006FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
     <author>Julien Schnitzler</author>
   </authors>
   <commentList>
-    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{C276C951-C1F7-40D1-A060-812AAFF9E361}">
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{C276C951-C1F7-40D1-A060-812AAFF9E361}">
       <text>
         <r>
           <rPr>
@@ -70,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{E7434F34-310B-4C48-87FC-7DD580B7051B}">
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{E7434F34-310B-4C48-87FC-7DD580B7051B}">
       <text>
         <r>
           <rPr>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="123">
   <si>
     <t>Titre</t>
   </si>
@@ -605,6 +605,24 @@
         ont déjà un emploi, mais en recherchent un autre
 </t>
     </r>
+  </si>
+  <si>
+    <t>Insee - Tableau de bord de l'économie française - TABLEAU DE BORD DE L'ÉCONOMIE FRANÇAISE</t>
+  </si>
+  <si>
+    <t>Taux de chômage en France par sexe et âge (INSEE)</t>
+  </si>
+  <si>
+    <t>TCSA</t>
+  </si>
+  <si>
+    <t>taux_chomage_sexe_age-insee-trimestriel-1975_2025.xlsx</t>
+  </si>
+  <si>
+    <t>Taux de chômage au sens du BIT (Bureau international du travail ) par sexe et tranches d'âge, parmis les 16-64 ans
+Note : données corrigées des variations saisonnières, en moyenne trimestrielle.				
+Lecture : au 4e trimestre 2025, le taux de chômage au sens du Bureau international du travail (BIT) des femmes est de 7,9 %. 				
+Champ : France hors Mayotte, personnes actives de 15 ans ou plus vivant en logement ordinaire.</t>
   </si>
 </sst>
 </file>
@@ -816,11 +834,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -848,18 +863,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -869,19 +876,108 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="15">
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <border outline="0">
         <top style="medium">
@@ -935,20 +1031,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{59FFD19D-A047-471C-9063-3B8296F55368}" name="Table1" displayName="Table1" ref="A1:K18" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A1:K18" xr:uid="{59FFD19D-A047-471C-9063-3B8296F55368}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{59FFD19D-A047-471C-9063-3B8296F55368}" name="Table1" displayName="Table1" ref="A1:K19" totalsRowShown="0" headerRowDxfId="14" dataDxfId="0" headerRowBorderDxfId="13" tableBorderDxfId="12">
+  <autoFilter ref="A1:K19" xr:uid="{59FFD19D-A047-471C-9063-3B8296F55368}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K19">
+    <sortCondition ref="J1:J19"/>
+  </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{5C6907E2-BCCE-4F36-BE87-40E3CE2282A0}" name="Titre"/>
-    <tableColumn id="8" xr3:uid="{7D19EA20-38D1-4D34-9BF1-AE9D5C98EF0B}" name="Abréviation"/>
-    <tableColumn id="9" xr3:uid="{D0434AC5-B08B-42D1-A4FB-10031603B067}" name="Présent"/>
-    <tableColumn id="2" xr3:uid="{492A637F-0C96-47AA-8B6E-D8212B39F7BD}" name="Description / Méthodologie"/>
-    <tableColumn id="3" xr3:uid="{F416C032-9509-4F4D-B0C6-4331470A61C0}" name="Source"/>
-    <tableColumn id="5" xr3:uid="{3A773317-8CEF-4E1A-9BB7-90871C273A1A}" name="URL de la source"/>
-    <tableColumn id="4" xr3:uid="{82F57AD2-7AEE-45F4-B019-B2130A51652B}" name="Attributs"/>
-    <tableColumn id="6" xr3:uid="{06B41314-6234-41A3-946F-BE91AB8B058A}" name="Fréquence"/>
-    <tableColumn id="10" xr3:uid="{89E3D434-6DE1-4BF4-BA81-753A36875736}" name="Date début"/>
-    <tableColumn id="11" xr3:uid="{7E23040E-882E-4EE9-B9A3-7A485BBE259A}" name="Date fin"/>
-    <tableColumn id="7" xr3:uid="{928910AA-F8E5-416F-BCC2-4DF0A8906CF0}" name="Nom du fichier dans data/raw"/>
+    <tableColumn id="1" xr3:uid="{5C6907E2-BCCE-4F36-BE87-40E3CE2282A0}" name="Titre" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{7D19EA20-38D1-4D34-9BF1-AE9D5C98EF0B}" name="Abréviation" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{D0434AC5-B08B-42D1-A4FB-10031603B067}" name="Présent" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{492A637F-0C96-47AA-8B6E-D8212B39F7BD}" name="Description / Méthodologie" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{F416C032-9509-4F4D-B0C6-4331470A61C0}" name="Source" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{3A773317-8CEF-4E1A-9BB7-90871C273A1A}" name="URL de la source" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{82F57AD2-7AEE-45F4-B019-B2130A51652B}" name="Attributs" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{06B41314-6234-41A3-946F-BE91AB8B058A}" name="Fréquence" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{89E3D434-6DE1-4BF4-BA81-753A36875736}" name="Date début" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{7E23040E-882E-4EE9-B9A3-7A485BBE259A}" name="Date fin" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{928910AA-F8E5-416F-BCC2-4DF0A8906CF0}" name="Nom du fichier dans data/raw" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1217,16 +1316,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K2" sqref="K2"/>
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40.81640625" customWidth="1"/>
+    <col min="1" max="1" width="43.90625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.54296875" customWidth="1"/>
     <col min="4" max="4" width="107.26953125" customWidth="1"/>
@@ -1238,620 +1337,654 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2" s="3" t="s">
+    <row r="2" spans="1:11" s="15" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="9" t="s">
+      <c r="D2" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="13">
+        <v>32874</v>
+      </c>
+      <c r="J2" s="13">
+        <v>45657</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="15" customFormat="1" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="23"/>
+      <c r="D3" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="G3" s="25"/>
+      <c r="H3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="18">
-        <v>35065</v>
-      </c>
-      <c r="J2" s="18">
-        <v>45838</v>
-      </c>
-      <c r="K2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="15" t="s">
+      <c r="I3" s="14">
+        <v>27395</v>
+      </c>
+      <c r="J3" s="14">
+        <v>46022</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="15" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="19">
-        <v>42005</v>
-      </c>
-      <c r="J3" s="20">
-        <v>45930</v>
-      </c>
-      <c r="K3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>108</v>
+      <c r="D4" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>109</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="18">
+      <c r="I4" s="14">
+        <v>27395</v>
+      </c>
+      <c r="J4" s="13">
+        <v>45657</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="15" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="25"/>
+      <c r="H5" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="I5" s="14">
+        <v>36161</v>
+      </c>
+      <c r="J5" s="32">
+        <v>45819</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="15" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="14">
+        <v>35065</v>
+      </c>
+      <c r="J6" s="13">
+        <v>45838</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="15" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="14">
+        <v>42005</v>
+      </c>
+      <c r="J7" s="32">
+        <v>45930</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="32">
+        <v>17899</v>
+      </c>
+      <c r="J8" s="32">
+        <v>45930</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="32">
+        <v>32143</v>
+      </c>
+      <c r="J9" s="32">
+        <v>45930</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="32">
+        <v>36526</v>
+      </c>
+      <c r="J10" s="32">
+        <v>45930</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="14">
         <v>32874</v>
       </c>
-      <c r="J4" s="18">
-        <v>45657</v>
-      </c>
-      <c r="K4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C5" s="16" t="s">
+      <c r="J11" s="14">
+        <v>45961</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="D5" t="s">
-        <v>113</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D12" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="14">
+        <v>32904</v>
+      </c>
+      <c r="J12" s="14">
+        <v>45961</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="G5" t="s">
-        <v>109</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="19">
-        <v>27395</v>
-      </c>
-      <c r="J5" s="18">
-        <v>45657</v>
-      </c>
-      <c r="K5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="15" t="s">
+      <c r="F13" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="14">
+        <v>33239</v>
+      </c>
+      <c r="J13" s="14">
+        <v>45991</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="10" t="s">
+      <c r="D14" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="19">
-        <v>32874</v>
-      </c>
-      <c r="J6" s="19">
-        <v>45961</v>
-      </c>
-      <c r="K6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="16" t="s">
+      <c r="I14" s="14">
+        <v>34365</v>
+      </c>
+      <c r="J14" s="14">
+        <v>46022</v>
+      </c>
+      <c r="K14" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="10" t="s">
+      <c r="D15" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="19">
-        <v>34365</v>
-      </c>
-      <c r="J7" s="19">
+      <c r="I15" s="14">
+        <v>33239</v>
+      </c>
+      <c r="J15" s="14">
         <v>46022</v>
       </c>
-      <c r="K7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="16" t="s">
+      <c r="K15" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="D8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" t="s">
-        <v>112</v>
-      </c>
-      <c r="I8" s="19">
-        <v>36161</v>
-      </c>
-      <c r="J8" s="20">
-        <v>45819</v>
-      </c>
-      <c r="K8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D16" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" s="14">
+        <v>33239</v>
+      </c>
+      <c r="J16" s="14">
+        <v>46022</v>
+      </c>
+      <c r="K16" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="D9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="D17" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" s="10" t="s">
+      <c r="F17" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="H17" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I17" s="14">
+        <v>28126</v>
+      </c>
+      <c r="J17" s="14">
+        <v>46022</v>
+      </c>
+      <c r="K17" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" s="14">
         <v>33239</v>
       </c>
-      <c r="J9" s="19">
+      <c r="J18" s="14">
         <v>46022</v>
       </c>
-      <c r="K9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="K18" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="D10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="D19" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" s="10" t="s">
+      <c r="F19" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="H19" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="19">
-        <v>33239</v>
-      </c>
-      <c r="J10" s="19">
-        <v>45991</v>
-      </c>
-      <c r="K10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I11" s="19">
-        <v>33239</v>
-      </c>
-      <c r="J11" s="19">
+      <c r="I19" s="14">
+        <v>32143</v>
+      </c>
+      <c r="J19" s="14">
         <v>46022</v>
       </c>
-      <c r="K11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B12" t="s">
-        <v>88</v>
-      </c>
-      <c r="C12" t="s">
-        <v>78</v>
-      </c>
-      <c r="D12" t="s">
-        <v>90</v>
-      </c>
-      <c r="E12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I12" s="19">
-        <v>28126</v>
-      </c>
-      <c r="J12" s="19">
-        <v>46022</v>
-      </c>
-      <c r="K12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="B13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C13" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" t="s">
-        <v>84</v>
-      </c>
-      <c r="E13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" s="19">
-        <v>33239</v>
-      </c>
-      <c r="J13" s="19">
-        <v>46022</v>
-      </c>
-      <c r="K13" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14" t="s">
-        <v>89</v>
-      </c>
-      <c r="C14" t="s">
-        <v>78</v>
-      </c>
-      <c r="D14" t="s">
-        <v>85</v>
-      </c>
-      <c r="E14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I14" s="19">
-        <v>32143</v>
-      </c>
-      <c r="J14" s="19">
-        <v>46022</v>
-      </c>
-      <c r="K14" t="s">
+      <c r="K19" s="15" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" t="s">
-        <v>78</v>
-      </c>
-      <c r="D15" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="H15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I15" s="20">
-        <v>17899</v>
-      </c>
-      <c r="J15" s="20">
-        <v>45930</v>
-      </c>
-      <c r="K15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="H16" t="s">
-        <v>13</v>
-      </c>
-      <c r="I16" s="20">
-        <v>32143</v>
-      </c>
-      <c r="J16" s="20">
-        <v>45930</v>
-      </c>
-      <c r="K16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" t="s">
-        <v>78</v>
-      </c>
-      <c r="D17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17" t="s">
-        <v>65</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I17" s="19">
-        <v>32904</v>
-      </c>
-      <c r="J17" s="19">
-        <v>45961</v>
-      </c>
-      <c r="K17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="B18" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" t="s">
-        <v>78</v>
-      </c>
-      <c r="D18" t="s">
-        <v>99</v>
-      </c>
-      <c r="E18" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="H18" t="s">
-        <v>13</v>
-      </c>
-      <c r="I18" s="20">
-        <v>36526</v>
-      </c>
-      <c r="J18" s="20">
-        <v>45930</v>
-      </c>
-      <c r="K18" t="s">
-        <v>72</v>
-      </c>
-    </row>
+    <row r="20" spans="1:11" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F6" r:id="rId1" xr:uid="{67742B9B-03CF-4FCB-9BCE-DE3B25272953}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{2EBCE280-964B-4B92-8D54-5F348CBCA2F5}"/>
-    <hyperlink ref="F16" r:id="rId3" location="Tableau" xr:uid="{645B4473-1C4E-40D1-8B1A-93EFDAFEB5A8}"/>
-    <hyperlink ref="F15" r:id="rId4" xr:uid="{50C517F9-015D-4A75-A453-055A876EE0EB}"/>
-    <hyperlink ref="F11" r:id="rId5" xr:uid="{BF31CC65-BB5C-45F3-9C22-A8EA69983D7C}"/>
-    <hyperlink ref="F10" r:id="rId6" xr:uid="{D3004A4A-3C06-4157-A56C-4F7B5BEBC346}"/>
-    <hyperlink ref="F9" r:id="rId7" xr:uid="{C4F79324-F5C2-4D69-B42C-10D939719E1B}"/>
-    <hyperlink ref="F8" r:id="rId8" display="https://data.ecb.europa.eu/data/datasets/FM/FM.B.U2.EUR.4F.KR.MRR_FR.LEV?chart_props=W3sibm9kZUlkIjoiMzQ2NTY5IiwicHJvcGVydGllcyI6W3siY29sb3JIZXgiOiIiLCJjb2xvclR5cGUiOiIiLCJjaGFydFR5cGUiOiJsaW5lY2hhcnQiLCJsaW5lU3R5bGUiOiJTb2xpZCIsImxpbmVXaWR0aCI6IjEuNSIsImF4aXNQb3NpdGlvbiI6ImxlZnQiLCJvYnNlcnZhdGlvblZhbHVlIjpmYWxzZSwiZGF0ZXMiOlsiMTk4MC0xMC0zMVQyMzowMDowMC4wMDBaIiwiMjAyNS0wNi0xMFQyMjowMDowMC4wMDBaIl0sImlzVGRhdGEiOmZhbHNlLCJtb2RpZmllZFVuaXRUeXBlIjoiIiwieWVhciI6Im9uZSIsInN0YXJ0RGF0ZSI6IjIwMjQtMDYtMTEiLCJlbmREYXRlIjoiMjAyNS0wNi0xMSIsInNldERhdGUiOnRydWUsInNob3dUYWJsZURhdGEiOmZhbHNlLCJjaGFuZ2VNb2RlIjpmYWxzZSwic2hvd01lbnVTdHlsZUNoYXJ0IjpmYWxzZSwiZGlzcGxheU1vYmlsZUNoYXJ0Ijp0cnVlLCJzY3JlZW5TaXplIjoibWF4Iiwic2NyZWVuV2lkdGgiOjE0NjEsInNob3dUZGF0YSI6ZmFsc2UsInRyYW5zZm9ybWVkRnJlcXVlbmN5Ijoibm9uZSIsInRyYW5zZm9ybWVkVW5pdCI6Im5vbmUiLCJmcmVxdWVuY3kiOiJub25lIiwidW5pdCI6Im5vbmUiLCJtb2RpZmllZCI6ImZhbHNlIiwic2VyaWVzS2V5IjoiZGFpbHkgLSBidXNpbmVzc3dlZWsiLCJzaG93dGFibGVTdGF0ZUJlZm9yZU1heFNjcmVlbiI6ZmFsc2UsImlzZGF0YWNvbXBhcmlzb24iOmZhbHNlLCJzZXJpZXNGcmVxdWVuY3kiOiJkYWlseSAtIGJ1c2luZXNzd2VlayIsImludGlhbFNlcmllc0ZyZXF1ZW5jeSI6ImRhaWx5IC0gYnVzaW5lc3N3ZWVrIiwibWV0YWRhdGFEZWNpbWFsIjoiNCIsImlzVGFibGVTb3J0ZWQiOmZhbHNlLCJpc1llYXJseVRkYXRhIjpmYWxzZSwicmVzcG9uc2VEYXRhRW5kRGF0ZSI6IjIwMjUtMDYtMTEiLCJpc2luaXRpYWxDaGFydERhdGEiOnRydWUsImlzRGF0ZXNGcm9tRGF0ZVBpY2tlciI6dHJ1ZSwiZGF0ZVBpY2tlckVuZERhdGUiOiIyMDI1LTA2LTExIiwiaXNEYXRlUGlja2VyRW5kRGF0ZSI6ZmFsc2UsInNlcmllc2tleVNldCI6IiIsImRhdGFzZXRJZCI6IjY3IiwiaXNDYWxsYmFjayI6ZmFsc2UsImlzU2xpZGVyVGRhdGEiOnRydWUsImlzU2xpZGVyRGF0YSI6dHJ1ZSwiaXNJbml0aWFsQ2hhcnREYXRhRnJvbUdyYXBoIjpmYWxzZSwiY2hhcnRTZXJpZXNLZXkiOiJGTS5CLlUyLkVVUi40Ri5LUi5NUlJfRlIuTEVWIiwidHlwZU9mIjoiIn1dfV0%3D" xr:uid="{5150F110-E71F-45AF-A510-1F71E4FD944C}"/>
-    <hyperlink ref="F7" r:id="rId9" display="https://data.ecb.europa.eu/data/datasets/FM/FM.M.U2.EUR.RT.MM.EURIBOR3MD_.HSTA?chart_props=W3sibm9kZUlkIjoiMzQ2NjQ3IiwicHJvcGVydGllcyI6W3siY29sb3JIZXgiOiIiLCJjb2xvclR5cGUiOiIiLCJjaGFydFR5cGUiOiJsaW5lY2hhcnQiLCJsaW5lU3R5bGUiOiJTb2xpZCIsImxpbmVXaWR0aCI6IjEuNSIsImF4aXNQb3NpdGlvbiI6ImxlZnQiLCJvYnNlcnZhdGlvblZhbHVlIjpmYWxzZSwiZGF0ZXMiOltdLCJpc1RkYXRhIjpmYWxzZSwibW9kaWZpZWRVbml0VHlwZSI6IiIsInllYXIiOiJmdWxsUmFuZ2UiLCJzdGFydERhdGUiOiIxOTk0LTAxLTMxIiwiZW5kRGF0ZSI6IjIwMjUtMTItMzEiLCJzZXREYXRlIjpmYWxzZSwic2hvd1RhYmxlRGF0YSI6dHJ1ZSwiY2hhbmdlTW9kZSI6ZmFsc2UsInNob3dNZW51U3R5bGVDaGFydCI6ZmFsc2UsImRpc3BsYXlNb2JpbGVDaGFydCI6dHJ1ZSwic2NyZWVuU2l6ZSI6Im1heCIsInNjcmVlbldpZHRoIjoxNDYxLCJzaG93VGRhdGEiOmZhbHNlLCJ0cmFuc2Zvcm1lZEZyZXF1ZW5jeSI6Im5vbmUiLCJ0cmFuc2Zvcm1lZFVuaXQiOiJub25lIiwiZnJlcXVlbmN5Ijoibm9uZSIsInVuaXQiOiJub25lIiwibW9kaWZpZWQiOiJmYWxzZSIsInNlcmllc0tleSI6Im1vbnRobHkiLCJzaG93dGFibGVTdGF0ZUJlZm9yZU1heFNjcmVlbiI6ZmFsc2UsImlzZGF0YWNvbXBhcmlzb24iOmZhbHNlLCJzZXJpZXNGcmVxdWVuY3kiOiJtb250aGx5IiwiaW50aWFsU2VyaWVzRnJlcXVlbmN5IjoibW9udGhseSIsIm1ldGFkYXRhRGVjaW1hbCI6IjQiLCJpc1RhYmxlU29ydGVkIjpmYWxzZSwiaXNZZWFybHlUZGF0YSI6ZmFsc2UsInJlc3BvbnNlRGF0YUVuZERhdGUiOiIyMDI1LTEyLTMxIiwiaXNpbml0aWFsQ2hhcnREYXRhIjp0cnVlLCJpc0RhdGVzRnJvbURhdGVQaWNrZXIiOmZhbHNlLCJkYXRlUGlja2VyRW5kRGF0ZSI6IiIsImlzRGF0ZVBpY2tlckVuZERhdGUiOmZhbHNlLCJzZXJpZXNrZXlTZXQiOiIiLCJkYXRhc2V0SWQiOiI2NyIsImlzQ2FsbGJhY2siOmZhbHNlLCJpc1NsaWRlclRkYXRhIjpmYWxzZSwiaXNTbGlkZXJEYXRhIjpmYWxzZSwiaXNJbml0aWFsQ2hhcnREYXRhRnJvbUdyYXBoIjpmYWxzZSwiY2hhcnRTZXJpZXNLZXkiOiJGTS5NLlUyLkVVUi5SVC5NTS5FVVJJQk9SM01EXy5IU1RBIiwidHlwZU9mIjoiIn1dfV0%3D" xr:uid="{9ABD0BA3-2276-42C7-AB83-0C545A545E03}"/>
-    <hyperlink ref="F17" r:id="rId10" xr:uid="{744E1553-15DB-4CBF-89A5-46E470D58578}"/>
-    <hyperlink ref="F18" r:id="rId11" xr:uid="{0B62988C-0924-419F-9185-AB42DB49E04E}"/>
-    <hyperlink ref="F2" r:id="rId12" xr:uid="{CC5EB80D-2561-413F-8F7D-91B9674F909E}"/>
+    <hyperlink ref="F11" r:id="rId1" xr:uid="{67742B9B-03CF-4FCB-9BCE-DE3B25272953}"/>
+    <hyperlink ref="F7" r:id="rId2" xr:uid="{2EBCE280-964B-4B92-8D54-5F348CBCA2F5}"/>
+    <hyperlink ref="F9" r:id="rId3" location="Tableau" xr:uid="{645B4473-1C4E-40D1-8B1A-93EFDAFEB5A8}"/>
+    <hyperlink ref="F8" r:id="rId4" xr:uid="{50C517F9-015D-4A75-A453-055A876EE0EB}"/>
+    <hyperlink ref="F16" r:id="rId5" xr:uid="{BF31CC65-BB5C-45F3-9C22-A8EA69983D7C}"/>
+    <hyperlink ref="F13" r:id="rId6" xr:uid="{D3004A4A-3C06-4157-A56C-4F7B5BEBC346}"/>
+    <hyperlink ref="F15" r:id="rId7" xr:uid="{C4F79324-F5C2-4D69-B42C-10D939719E1B}"/>
+    <hyperlink ref="F5" r:id="rId8" display="https://data.ecb.europa.eu/data/datasets/FM/FM.B.U2.EUR.4F.KR.MRR_FR.LEV?chart_props=W3sibm9kZUlkIjoiMzQ2NTY5IiwicHJvcGVydGllcyI6W3siY29sb3JIZXgiOiIiLCJjb2xvclR5cGUiOiIiLCJjaGFydFR5cGUiOiJsaW5lY2hhcnQiLCJsaW5lU3R5bGUiOiJTb2xpZCIsImxpbmVXaWR0aCI6IjEuNSIsImF4aXNQb3NpdGlvbiI6ImxlZnQiLCJvYnNlcnZhdGlvblZhbHVlIjpmYWxzZSwiZGF0ZXMiOlsiMTk4MC0xMC0zMVQyMzowMDowMC4wMDBaIiwiMjAyNS0wNi0xMFQyMjowMDowMC4wMDBaIl0sImlzVGRhdGEiOmZhbHNlLCJtb2RpZmllZFVuaXRUeXBlIjoiIiwieWVhciI6Im9uZSIsInN0YXJ0RGF0ZSI6IjIwMjQtMDYtMTEiLCJlbmREYXRlIjoiMjAyNS0wNi0xMSIsInNldERhdGUiOnRydWUsInNob3dUYWJsZURhdGEiOmZhbHNlLCJjaGFuZ2VNb2RlIjpmYWxzZSwic2hvd01lbnVTdHlsZUNoYXJ0IjpmYWxzZSwiZGlzcGxheU1vYmlsZUNoYXJ0Ijp0cnVlLCJzY3JlZW5TaXplIjoibWF4Iiwic2NyZWVuV2lkdGgiOjE0NjEsInNob3dUZGF0YSI6ZmFsc2UsInRyYW5zZm9ybWVkRnJlcXVlbmN5Ijoibm9uZSIsInRyYW5zZm9ybWVkVW5pdCI6Im5vbmUiLCJmcmVxdWVuY3kiOiJub25lIiwidW5pdCI6Im5vbmUiLCJtb2RpZmllZCI6ImZhbHNlIiwic2VyaWVzS2V5IjoiZGFpbHkgLSBidXNpbmVzc3dlZWsiLCJzaG93dGFibGVTdGF0ZUJlZm9yZU1heFNjcmVlbiI6ZmFsc2UsImlzZGF0YWNvbXBhcmlzb24iOmZhbHNlLCJzZXJpZXNGcmVxdWVuY3kiOiJkYWlseSAtIGJ1c2luZXNzd2VlayIsImludGlhbFNlcmllc0ZyZXF1ZW5jeSI6ImRhaWx5IC0gYnVzaW5lc3N3ZWVrIiwibWV0YWRhdGFEZWNpbWFsIjoiNCIsImlzVGFibGVTb3J0ZWQiOmZhbHNlLCJpc1llYXJseVRkYXRhIjpmYWxzZSwicmVzcG9uc2VEYXRhRW5kRGF0ZSI6IjIwMjUtMDYtMTEiLCJpc2luaXRpYWxDaGFydERhdGEiOnRydWUsImlzRGF0ZXNGcm9tRGF0ZVBpY2tlciI6dHJ1ZSwiZGF0ZVBpY2tlckVuZERhdGUiOiIyMDI1LTA2LTExIiwiaXNEYXRlUGlja2VyRW5kRGF0ZSI6ZmFsc2UsInNlcmllc2tleVNldCI6IiIsImRhdGFzZXRJZCI6IjY3IiwiaXNDYWxsYmFjayI6ZmFsc2UsImlzU2xpZGVyVGRhdGEiOnRydWUsImlzU2xpZGVyRGF0YSI6dHJ1ZSwiaXNJbml0aWFsQ2hhcnREYXRhRnJvbUdyYXBoIjpmYWxzZSwiY2hhcnRTZXJpZXNLZXkiOiJGTS5CLlUyLkVVUi40Ri5LUi5NUlJfRlIuTEVWIiwidHlwZU9mIjoiIn1dfV0%3D" xr:uid="{5150F110-E71F-45AF-A510-1F71E4FD944C}"/>
+    <hyperlink ref="F14" r:id="rId9" display="https://data.ecb.europa.eu/data/datasets/FM/FM.M.U2.EUR.RT.MM.EURIBOR3MD_.HSTA?chart_props=W3sibm9kZUlkIjoiMzQ2NjQ3IiwicHJvcGVydGllcyI6W3siY29sb3JIZXgiOiIiLCJjb2xvclR5cGUiOiIiLCJjaGFydFR5cGUiOiJsaW5lY2hhcnQiLCJsaW5lU3R5bGUiOiJTb2xpZCIsImxpbmVXaWR0aCI6IjEuNSIsImF4aXNQb3NpdGlvbiI6ImxlZnQiLCJvYnNlcnZhdGlvblZhbHVlIjpmYWxzZSwiZGF0ZXMiOltdLCJpc1RkYXRhIjpmYWxzZSwibW9kaWZpZWRVbml0VHlwZSI6IiIsInllYXIiOiJmdWxsUmFuZ2UiLCJzdGFydERhdGUiOiIxOTk0LTAxLTMxIiwiZW5kRGF0ZSI6IjIwMjUtMTItMzEiLCJzZXREYXRlIjpmYWxzZSwic2hvd1RhYmxlRGF0YSI6dHJ1ZSwiY2hhbmdlTW9kZSI6ZmFsc2UsInNob3dNZW51U3R5bGVDaGFydCI6ZmFsc2UsImRpc3BsYXlNb2JpbGVDaGFydCI6dHJ1ZSwic2NyZWVuU2l6ZSI6Im1heCIsInNjcmVlbldpZHRoIjoxNDYxLCJzaG93VGRhdGEiOmZhbHNlLCJ0cmFuc2Zvcm1lZEZyZXF1ZW5jeSI6Im5vbmUiLCJ0cmFuc2Zvcm1lZFVuaXQiOiJub25lIiwiZnJlcXVlbmN5Ijoibm9uZSIsInVuaXQiOiJub25lIiwibW9kaWZpZWQiOiJmYWxzZSIsInNlcmllc0tleSI6Im1vbnRobHkiLCJzaG93dGFibGVTdGF0ZUJlZm9yZU1heFNjcmVlbiI6ZmFsc2UsImlzZGF0YWNvbXBhcmlzb24iOmZhbHNlLCJzZXJpZXNGcmVxdWVuY3kiOiJtb250aGx5IiwiaW50aWFsU2VyaWVzRnJlcXVlbmN5IjoibW9udGhseSIsIm1ldGFkYXRhRGVjaW1hbCI6IjQiLCJpc1RhYmxlU29ydGVkIjpmYWxzZSwiaXNZZWFybHlUZGF0YSI6ZmFsc2UsInJlc3BvbnNlRGF0YUVuZERhdGUiOiIyMDI1LTEyLTMxIiwiaXNpbml0aWFsQ2hhcnREYXRhIjp0cnVlLCJpc0RhdGVzRnJvbURhdGVQaWNrZXIiOmZhbHNlLCJkYXRlUGlja2VyRW5kRGF0ZSI6IiIsImlzRGF0ZVBpY2tlckVuZERhdGUiOmZhbHNlLCJzZXJpZXNrZXlTZXQiOiIiLCJkYXRhc2V0SWQiOiI2NyIsImlzQ2FsbGJhY2siOmZhbHNlLCJpc1NsaWRlclRkYXRhIjpmYWxzZSwiaXNTbGlkZXJEYXRhIjpmYWxzZSwiaXNJbml0aWFsQ2hhcnREYXRhRnJvbUdyYXBoIjpmYWxzZSwiY2hhcnRTZXJpZXNLZXkiOiJGTS5NLlUyLkVVUi5SVC5NTS5FVVJJQk9SM01EXy5IU1RBIiwidHlwZU9mIjoiIn1dfV0%3D" xr:uid="{9ABD0BA3-2276-42C7-AB83-0C545A545E03}"/>
+    <hyperlink ref="F12" r:id="rId10" xr:uid="{744E1553-15DB-4CBF-89A5-46E470D58578}"/>
+    <hyperlink ref="F10" r:id="rId11" xr:uid="{0B62988C-0924-419F-9185-AB42DB49E04E}"/>
+    <hyperlink ref="F6" r:id="rId12" xr:uid="{CC5EB80D-2561-413F-8F7D-91B9674F909E}"/>
+    <hyperlink ref="F3" r:id="rId13" display="https://www.insee.fr/fr/outil-interactif/5367857/tableau/50_MTS/52_CHO" xr:uid="{DB198841-507D-4B5B-9C0B-8DDFA5B229B6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
-  <legacyDrawing r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <legacyDrawing r:id="rId15"/>
   <tableParts count="1">
-    <tablePart r:id="rId15"/>
+    <tablePart r:id="rId16"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1871,26 +2004,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="10" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="408" x14ac:dyDescent="0.35">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="16" t="s">
         <v>117</v>
       </c>
     </row>

</xml_diff>